<commit_message>
committing all the changes
</commit_message>
<xml_diff>
--- a/TestData/ProductCPSearch.xlsx
+++ b/TestData/ProductCPSearch.xlsx
@@ -31,9 +31,6 @@
     <t>https://www.syngenta.it/prodotti/cerca/protezione-colture</t>
   </si>
   <si>
-    <t>https://www.syngenta.bg/bg/products/search/crop-protection</t>
-  </si>
-  <si>
     <t>https://www.syngenta.fr/produits/recherche</t>
   </si>
   <si>
@@ -128,6 +125,9 @@
   </si>
   <si>
     <t>https://www.syngenta.si/products/search/crop-protection</t>
+  </si>
+  <si>
+    <t>https://www.syngenta.bg/products/search/crop-protection</t>
   </si>
 </sst>
 </file>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,167 +518,167 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>